<commit_message>
Added Burndown List for NetVecCad basics
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CadObjectHierarchy" sheetId="1" r:id="rId1"/>
     <sheet name="FeatureAndSymbology" sheetId="4" r:id="rId2"/>
     <sheet name="CommandClass" sheetId="5" r:id="rId3"/>
+    <sheet name="BurnDownList" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -21,7 +22,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E10" authorId="0">
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -29,7 +30,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -38,7 +39,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Point Origin;
@@ -49,7 +50,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="F12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -66,7 +67,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Double Height;
@@ -74,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="119">
   <si>
     <t>Comment</t>
   </si>
@@ -319,26 +320,159 @@
     <t>NVcad color</t>
   </si>
   <si>
-    <t>BackgroundColor</t>
-  </si>
-  <si>
-    <t>BackgroundTransparency</t>
-  </si>
-  <si>
-    <t>1.0 = 100% Transparent, which is the default</t>
-  </si>
-  <si>
     <t>BackgroundMargin</t>
   </si>
   <si>
     <t>0.1 = 10% of FontSize</t>
+  </si>
+  <si>
+    <t>Interfaces</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>FillColor</t>
+  </si>
+  <si>
+    <t>FillTransparency</t>
+  </si>
+  <si>
+    <t>Applicable only to shapes and text</t>
+  </si>
+  <si>
+    <t>IBoundingBoxed</t>
+  </si>
+  <si>
+    <t>Text has background when BackgroundMargin is not null.  FillColor and FillTransparency are used</t>
+  </si>
+  <si>
+    <t>to control background appearance of the text.</t>
+  </si>
+  <si>
+    <t>Is a list of Commands.  May be bookmarked or saved</t>
+  </si>
+  <si>
+    <t>Software Item</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Line in Model draws on View</t>
+  </si>
+  <si>
+    <t>NVCadView View (inherits from Canvas)</t>
+  </si>
+  <si>
+    <t>Text in Model draws on View</t>
+  </si>
+  <si>
+    <t>MouseOver shows world coordinates</t>
+  </si>
+  <si>
+    <t>Arc in model draws on View</t>
+  </si>
+  <si>
+    <t>MouseDrag slides View</t>
+  </si>
+  <si>
+    <t>Completion Status</t>
+  </si>
+  <si>
+    <t>Test Coverage</t>
+  </si>
+  <si>
+    <t>Time Estimate</t>
+  </si>
+  <si>
+    <t>Total Time</t>
+  </si>
+  <si>
+    <t>Fit View Command</t>
+  </si>
+  <si>
+    <t>Zoom View</t>
+  </si>
+  <si>
+    <t>Apply Features to Elements</t>
+  </si>
+  <si>
+    <t>Show Flyover Data</t>
+  </si>
+  <si>
+    <t>Date Estimate</t>
+  </si>
+  <si>
+    <t>Actual Date</t>
+  </si>
+  <si>
+    <t>Load .dxf into model</t>
+  </si>
+  <si>
+    <t>Display model populated by .dxf</t>
+  </si>
+  <si>
+    <t>Keyin Window (minimal functionality)</t>
+  </si>
+  <si>
+    <t>Place Line command, xy=, dl= (no dynamics)</t>
+  </si>
+  <si>
+    <t>Place arcPt3 command</t>
+  </si>
+  <si>
+    <t>Persist Model as OpenOffice document</t>
+  </si>
+  <si>
+    <t>Named Groups with nesting</t>
+  </si>
+  <si>
+    <t>Add to Named Group keyin</t>
+  </si>
+  <si>
+    <t>Place Line and Arc icons on a toolbar</t>
+  </si>
+  <si>
+    <t>Move Element</t>
+  </si>
+  <si>
+    <t>Copy Element</t>
+  </si>
+  <si>
+    <t>Get/Set Symbology</t>
+  </si>
+  <si>
+    <t>Delete Element</t>
+  </si>
+  <si>
+    <t>Undo/Redo</t>
+  </si>
+  <si>
+    <t>Export to dxf format</t>
+  </si>
+  <si>
+    <t>Interactive Parameters Window</t>
+  </si>
+  <si>
+    <t>Print View to pdf</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>perfect projection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="[h]:mm"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0#&quot; mandays&quot;"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,19 +493,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
@@ -419,13 +540,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -729,11 +863,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,21 +881,22 @@
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.109375" customWidth="1"/>
     <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -789,8 +924,11 @@
       <c r="I4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>0.1</v>
       </c>
@@ -798,7 +936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>0</v>
       </c>
@@ -806,7 +944,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -816,8 +954,11 @@
       <c r="F7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>0</v>
       </c>
@@ -825,7 +966,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>81</v>
+      </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
@@ -833,88 +977,91 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>0</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="3">
+      <c r="K11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
         <v>0.1</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="3">
-        <v>0</v>
-      </c>
-      <c r="C12">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>0</v>
+      </c>
+      <c r="C13">
         <v>7</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="3">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
         <v>0.01</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>2</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H16" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
-        <v>0</v>
+        <v>0.01</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -922,7 +1069,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -930,26 +1077,23 @@
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <v>0</v>
       </c>
-      <c r="H21" t="s">
-        <v>23</v>
+      <c r="I21" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <v>0</v>
       </c>
-      <c r="C22">
-        <v>101</v>
-      </c>
-      <c r="G22" t="s">
-        <v>65</v>
+      <c r="H22" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -957,54 +1101,54 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <v>0</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="C24">
+        <v>102</v>
+      </c>
+      <c r="G24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="3">
-        <v>0</v>
-      </c>
-      <c r="C26">
+      <c r="B27" s="3">
+        <v>0</v>
+      </c>
+      <c r="C27">
         <v>6</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27">
-        <v>4</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1012,21 +1156,46 @@
         <v>0</v>
       </c>
       <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29">
         <v>5</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="B30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34">
+        <v>1.5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1038,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1158,82 +1327,94 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>39</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>54</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>59</v>
       </c>
       <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" t="s">
-        <v>75</v>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1251,4 +1432,528 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.77734375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="7"/>
+    <col min="3" max="3" width="20.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="11">
+        <f>SUM(E4:E2000)*24/8</f>
+        <v>38.25</v>
+      </c>
+      <c r="F1" s="8">
+        <f>DATE(2014,4,21)+(CEILING(SUM(E4:E2000)*24/8,1)*7/5)</f>
+        <v>41804.6</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="12">
+        <f>CEILING(SUM(E4:E2000)*24/8,1)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>1.25</v>
+      </c>
+      <c r="F4" s="8">
+        <v>41759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="8">
+        <v>41760</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="7">
+        <v>3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F6" s="8">
+        <v>41761</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F7" s="8">
+        <v>41765</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="7">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F8" s="8">
+        <v>41766</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="7">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="8">
+        <v>41767</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="7">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F10" s="8">
+        <v>41768</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="7">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0</v>
+      </c>
+      <c r="E11" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F11" s="8">
+        <v>41769</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="7">
+        <v>9</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="8">
+        <v>41772</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>97</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F13" s="8">
+        <v>41772</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="7">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F14" s="8">
+        <v>41773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="7">
+        <v>12</v>
+      </c>
+      <c r="C15" s="6">
+        <v>0</v>
+      </c>
+      <c r="E15" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F15" s="8">
+        <v>41773</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" s="7">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0</v>
+      </c>
+      <c r="E16" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F16" s="8">
+        <v>41774</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="7">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F17" s="8">
+        <v>41778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="7">
+        <v>15</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="8">
+        <v>41781</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="7">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F19" s="8">
+        <v>41786</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>105</v>
+      </c>
+      <c r="B20" s="7">
+        <v>17</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F20" s="8">
+        <v>41793</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21" s="7">
+        <v>18</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F21" s="8">
+        <v>41794</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B22" s="7">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="7">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F23" s="8">
+        <v>41799</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="7">
+        <v>20</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F24" s="8">
+        <v>41799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" s="7">
+        <v>21</v>
+      </c>
+      <c r="C25" s="6">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F25" s="8">
+        <v>41800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>111</v>
+      </c>
+      <c r="B26" s="7">
+        <v>22</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="F26" s="8">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>112</v>
+      </c>
+      <c r="B27" s="7">
+        <v>23</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0</v>
+      </c>
+      <c r="E27" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F27" s="8">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="7">
+        <v>24</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>41806</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="7">
+        <v>25</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F29" s="8">
+        <v>41809</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" s="7">
+        <v>26</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F30" s="8">
+        <v>41813</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Burndown List: Updated Format and progress
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -13,6 +13,7 @@
     <sheet name="BurnDownList" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -473,7 +474,7 @@
     <t>ArchimedesSpiral</t>
   </si>
   <si>
-    <t>As of 4/23</t>
+    <t>As of 5/2</t>
   </si>
 </sst>
 </file>
@@ -558,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -577,7 +578,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1471,12 +1471,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:Y30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,10 +1491,11 @@
     <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="9" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
-    <col min="9" max="9" width="38.109375" customWidth="1"/>
+    <col min="9" max="9" width="32.88671875" customWidth="1"/>
+    <col min="10" max="25" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
         <v>116</v>
       </c>
@@ -1507,9 +1510,8 @@
       <c r="G1" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="12"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>82</v>
       </c>
@@ -1538,32 +1540,61 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
-        <v>0</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="16">
+      <c r="C4" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15">
         <v>1.25</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>41759</v>
       </c>
-      <c r="G4" s="16">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="H4" s="17"/>
-      <c r="I4" s="13" t="s">
+      <c r="G4" s="15">
+        <f>SUM(J4:Y4)</f>
+        <v>0.8652777777777777</v>
+      </c>
+      <c r="H4" s="16"/>
+      <c r="I4" s="12" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J4" s="15">
+        <v>5.9027777777777783E-2</v>
+      </c>
+      <c r="K4" s="15">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="L4" s="15">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="M4" s="15">
+        <v>0.23124999999999998</v>
+      </c>
+      <c r="N4" s="15">
+        <v>0.29375000000000001</v>
+      </c>
+      <c r="O4" s="15">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
+      <c r="W4" s="15"/>
+      <c r="X4" s="15"/>
+      <c r="Y4" s="15"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1580,7 +1611,7 @@
         <v>41760</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -1597,7 +1628,7 @@
         <v>41761</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>87</v>
       </c>
@@ -1614,7 +1645,7 @@
         <v>41765</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>88</v>
       </c>
@@ -1631,7 +1662,7 @@
         <v>41766</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>89</v>
       </c>
@@ -1648,7 +1679,7 @@
         <v>41767</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -1665,7 +1696,7 @@
         <v>41768</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -1682,7 +1713,7 @@
         <v>41769</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -1699,7 +1730,7 @@
         <v>41772</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -1716,7 +1747,7 @@
         <v>41772</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>100</v>
       </c>
@@ -1733,7 +1764,7 @@
         <v>41773</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>101</v>
       </c>
@@ -1750,7 +1781,7 @@
         <v>41773</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>102</v>
       </c>
@@ -2004,5 +2035,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ViewCanvas: Added ability for model to draw line
Added ability for model to draw lines on a ViewCanvas.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -474,16 +474,17 @@
     <t>ArchimedesSpiral</t>
   </si>
   <si>
-    <t>As of 5/2</t>
+    <t>Implement View class in Model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="#,##0.0#&quot; mandays&quot;"/>
+    <numFmt numFmtId="166" formatCode="[h]:mm;;"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -559,7 +560,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -587,6 +588,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1471,14 +1484,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1489,7 +1502,7 @@
     <col min="4" max="4" width="16.5546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" style="22" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="32.88671875" customWidth="1"/>
     <col min="10" max="25" width="8.88671875" style="9"/>
@@ -1500,14 +1513,14 @@
         <v>116</v>
       </c>
       <c r="E1" s="11">
-        <f>SUM(E4:E2000)*24/8</f>
+        <f>SUM(E4:E2001)*24/8</f>
         <v>38.25</v>
       </c>
       <c r="F1" s="8">
-        <f>DATE(2014,4,21)+(CEILING(SUM(E4:E2000)*24/8,1)*7/5)</f>
+        <f>DATE(2014,4,21)+(CEILING(SUM(E4:E2001)*24/8,1)*7/5)</f>
         <v>41804.6</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="22" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1530,7 +1543,7 @@
       <c r="F3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="22" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1540,76 +1553,103 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15">
+      <c r="C4" s="19">
+        <v>1</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20">
         <v>1.25</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="21">
         <v>41759</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="23">
         <f>SUM(J4:Y4)</f>
-        <v>0.8652777777777777</v>
-      </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" s="15">
+        <v>0.89097222222222217</v>
+      </c>
+      <c r="H4" s="21">
+        <v>41762</v>
+      </c>
+      <c r="J4" s="20">
         <v>5.9027777777777783E-2</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="20">
         <v>6.1111111111111116E-2</v>
       </c>
-      <c r="L4" s="15">
+      <c r="L4" s="20">
         <v>5.347222222222222E-2</v>
       </c>
-      <c r="M4" s="15">
+      <c r="M4" s="20">
         <v>0.23124999999999998</v>
       </c>
-      <c r="N4" s="15">
+      <c r="N4" s="20">
         <v>0.29375000000000001</v>
       </c>
-      <c r="O4" s="15">
+      <c r="O4" s="20">
         <v>0.16666666666666666</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="P4" s="20">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="20"/>
+      <c r="Y4" s="20"/>
+    </row>
+    <row r="5" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="C5" s="14">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15">
         <v>0.25</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="16">
         <v>41760</v>
       </c>
+      <c r="G5" s="24">
+        <f>SUM(J5:Y5)</f>
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="H5" s="16">
+        <v>41762</v>
+      </c>
+      <c r="J5" s="15">
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1627,316 +1667,392 @@
       <c r="F6" s="8">
         <v>41761</v>
       </c>
+      <c r="G6" s="22">
+        <f>SUM(J6:Y6)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>122</v>
       </c>
       <c r="B7" s="7">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C7" s="6">
         <v>0</v>
       </c>
       <c r="E7" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.20833333333333334</v>
       </c>
       <c r="F7" s="8">
-        <v>41765</v>
+        <v>41764</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" ref="G7:G31" si="0">SUM(J7:Y7)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="6">
         <v>0</v>
       </c>
       <c r="E8" s="9">
-        <v>0.33333333333333331</v>
+        <v>0.125</v>
       </c>
       <c r="F8" s="8">
-        <v>41766</v>
+        <v>41765</v>
+      </c>
+      <c r="G8" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6">
         <v>0</v>
       </c>
       <c r="E9" s="9">
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F9" s="8">
-        <v>41767</v>
+        <v>41766</v>
+      </c>
+      <c r="G9" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B10" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="6">
         <v>0</v>
       </c>
       <c r="E10" s="9">
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="F10" s="8">
-        <v>41768</v>
+        <v>41767</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
       </c>
       <c r="E11" s="9">
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F11" s="8">
-        <v>41769</v>
+        <v>41768</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="6">
         <v>0</v>
       </c>
       <c r="E12" s="9">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F12" s="8">
-        <v>41772</v>
+        <v>41769</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="6">
         <v>0</v>
       </c>
       <c r="E13" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="8">
         <v>41772</v>
       </c>
+      <c r="G13" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B14" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
       </c>
       <c r="E14" s="9">
-        <v>0.33333333333333331</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F14" s="8">
-        <v>41773</v>
+        <v>41772</v>
+      </c>
+      <c r="G14" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="6">
         <v>0</v>
       </c>
       <c r="E15" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F15" s="8">
         <v>41773</v>
       </c>
+      <c r="G15" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F16" s="8">
-        <v>41774</v>
+        <v>41773</v>
+      </c>
+      <c r="G16" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
       </c>
       <c r="E17" s="9">
-        <v>0.66666666666666663</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F17" s="8">
-        <v>41778</v>
+        <v>41774</v>
+      </c>
+      <c r="G17" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B18" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="6">
         <v>0</v>
       </c>
       <c r="E18" s="9">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F18" s="8">
-        <v>41781</v>
-      </c>
-      <c r="I18" t="s">
-        <v>120</v>
+        <v>41778</v>
+      </c>
+      <c r="G18" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B19" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
       </c>
       <c r="E19" s="9">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="F19" s="8">
-        <v>41786</v>
+        <v>41781</v>
+      </c>
+      <c r="G19" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="6">
         <v>0</v>
       </c>
       <c r="E20" s="9">
-        <v>1.6666666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F20" s="8">
-        <v>41793</v>
+        <v>41786</v>
+      </c>
+      <c r="G20" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B21" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="6">
         <v>0</v>
       </c>
       <c r="E21" s="9">
-        <v>0.33333333333333331</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F21" s="8">
-        <v>41794</v>
+        <v>41793</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B22" s="7">
-        <v>1000</v>
+        <v>18</v>
       </c>
       <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F22" s="8">
+        <v>41794</v>
+      </c>
+      <c r="G22" s="22">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B23" s="7">
-        <v>19</v>
+        <v>1000</v>
       </c>
       <c r="C23" s="6">
         <v>0</v>
       </c>
-      <c r="E23" s="9">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F23" s="8">
-        <v>41799</v>
+      <c r="G23" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B24" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24" s="6">
         <v>0</v>
       </c>
       <c r="E24" s="9">
-        <v>0.16666666666666666</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F24" s="8">
         <v>41799</v>
       </c>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B25" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25" s="6">
         <v>0</v>
@@ -1945,92 +2061,137 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F25" s="8">
-        <v>41800</v>
+        <v>41799</v>
+      </c>
+      <c r="G25" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B26" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" s="6">
         <v>0</v>
       </c>
       <c r="E26" s="9">
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F26" s="8">
-        <v>41801</v>
+        <v>41800</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C27" s="6">
         <v>0</v>
       </c>
       <c r="E27" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F27" s="8">
         <v>41801</v>
       </c>
+      <c r="G27" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B28" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="6">
         <v>0</v>
       </c>
       <c r="E28" s="9">
-        <v>1</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F28" s="8">
-        <v>41806</v>
+        <v>41801</v>
+      </c>
+      <c r="G28" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C29" s="6">
         <v>0</v>
       </c>
       <c r="E29" s="9">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="F29" s="8">
-        <v>41809</v>
+        <v>41806</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" s="7">
+        <v>25</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0</v>
+      </c>
+      <c r="E30" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F30" s="8">
+        <v>41809</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B31" s="7">
         <v>26</v>
       </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-      <c r="E30" s="9">
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="E31" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F31" s="8">
         <v>41813</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
View Canvas: Worked on rotated text
Could not get rotated text to work.  Time to move on.  Will return to
this later.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="124">
   <si>
     <t>Comment</t>
   </si>
@@ -475,6 +475,9 @@
   </si>
   <si>
     <t>Implement View class in Model</t>
+  </si>
+  <si>
+    <t>Just can't get rotated text to work.</t>
   </si>
 </sst>
 </file>
@@ -1487,11 +1490,11 @@
   <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,69 +1611,96 @@
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
     </row>
-    <row r="5" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="18">
         <v>2</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="19">
         <v>1</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15">
+      <c r="D5" s="19"/>
+      <c r="E5" s="20">
         <v>0.25</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="21">
         <v>41760</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <f>SUM(J5:Y5)</f>
         <v>7.3611111111111113E-2</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="21">
         <v>41762</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="20">
         <v>7.3611111111111113E-2</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="15"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+    </row>
+    <row r="6" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
+      <c r="C6" s="14">
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="15">
         <v>0.25</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="16">
         <v>41761</v>
       </c>
-      <c r="G6" s="22">
+      <c r="G6" s="24">
         <f>SUM(J6:Y6)</f>
-        <v>0</v>
-      </c>
+        <v>0.2013888888888889</v>
+      </c>
+      <c r="H6" s="16">
+        <v>41762</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="15">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="K6" s="15">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">

</xml_diff>

<commit_message>
Text now draws correctly, including rotated text
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="127">
   <si>
     <t>Comment</t>
   </si>
@@ -480,6 +480,12 @@
   </si>
   <si>
     <t>Rotated views: elements, coordinate xfrms</t>
+  </si>
+  <si>
+    <t>Task morphed into implementing child windows</t>
+  </si>
+  <si>
+    <t>Reimpliment Text draws on View</t>
   </si>
 </sst>
 </file>
@@ -527,7 +533,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,12 +556,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -571,7 +571,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -611,16 +611,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1505,14 +1497,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,23 +1521,23 @@
     <col min="10" max="25" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
         <v>116</v>
       </c>
       <c r="E1" s="11">
-        <f>SUM(E4:E2002)*24/8</f>
-        <v>39.25</v>
+        <f>SUM(E4:E2003)*24/8</f>
+        <v>42.5</v>
       </c>
       <c r="F1" s="8">
-        <f>DATE(2014,4,21)+(CEILING(SUM(E4:E2002)*24/8,1)*7/5)</f>
-        <v>41806</v>
+        <f>DATE(2014,4,21)+(CEILING(SUM(E4:E2003)*24/8,1)*7/5)</f>
+        <v>41810.199999999997</v>
       </c>
       <c r="G1" s="22" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>82</v>
       </c>
@@ -1574,7 +1566,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>85</v>
       </c>
@@ -1629,7 +1621,7 @@
       <c r="X4" s="20"/>
       <c r="Y4" s="20"/>
     </row>
-    <row r="5" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>84</v>
       </c>
@@ -1672,288 +1664,345 @@
       <c r="X5" s="20"/>
       <c r="Y5" s="20"/>
     </row>
-    <row r="6" spans="1:25" s="25" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="18">
         <v>3</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="19">
         <v>0.9</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28">
+      <c r="D6" s="19"/>
+      <c r="E6" s="20">
         <v>0.25</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="21">
         <v>41761</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="23">
         <f>SUM(J6:Y6)</f>
         <v>0.2013888888888889</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="21">
         <v>41762</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="28">
+      <c r="J6" s="20">
         <v>0.17361111111111113</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="20">
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-    </row>
-    <row r="7" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+    </row>
+    <row r="7" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="18">
         <v>3.5</v>
       </c>
-      <c r="C7" s="14">
-        <v>0.35</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15">
+      <c r="C7" s="19">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="21">
         <v>41764</v>
       </c>
-      <c r="G7" s="24">
-        <f t="shared" ref="G7:G32" si="0">SUM(J7:Y7)</f>
-        <v>0.31458333333333333</v>
-      </c>
-      <c r="H7" s="16">
-        <v>41765</v>
-      </c>
-      <c r="J7" s="15">
+      <c r="G7" s="23">
+        <f>SUM(J7:AZ7)</f>
+        <v>1.0923611111111111</v>
+      </c>
+      <c r="H7" s="21">
+        <v>41793</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="20">
         <v>6.25E-2</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K7" s="20">
         <v>3.6805555555555557E-2</v>
       </c>
-      <c r="L7" s="15">
+      <c r="L7" s="20">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="M7" s="15">
+      <c r="M7" s="20">
         <v>3.125E-2</v>
       </c>
-      <c r="N7" s="15">
+      <c r="N7" s="20">
         <v>7.013888888888889E-2</v>
       </c>
-      <c r="O7" s="15">
+      <c r="O7" s="20">
         <v>2.5694444444444447E-2</v>
       </c>
-      <c r="P7" s="15">
-        <v>4.6527777777777779E-2</v>
-      </c>
-      <c r="Q7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="P7" s="20">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="R7" s="20">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="S7" s="20">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="T7" s="20">
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="U7" s="20">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="V7" s="20">
+        <v>0.21388888888888891</v>
+      </c>
+      <c r="W7" s="20">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="X7" s="20">
+        <v>0.13749999999999998</v>
+      </c>
+      <c r="Y7" s="20">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="Z7" s="26">
+        <v>4.5138888888888888E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="13">
+        <v>3.6</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="15">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F8" s="16">
+        <v>41794</v>
+      </c>
+      <c r="G8" s="24">
+        <f>SUM(J8:AZ8)</f>
+        <v>0.11180555555555555</v>
+      </c>
+      <c r="H8" s="16">
+        <v>41794</v>
+      </c>
+      <c r="J8" s="15">
+        <v>6.25E-2</v>
+      </c>
+      <c r="K8" s="15">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="25"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>87</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B9" s="7">
         <v>4</v>
       </c>
-      <c r="C8" s="6">
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F8" s="8">
-        <v>41765</v>
-      </c>
-      <c r="G8" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="F9" s="8">
+        <f>F8+1</f>
+        <v>41795</v>
+      </c>
+      <c r="G9" s="22">
+        <f t="shared" ref="G9:G33" si="0">SUM(J9:Y9)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B10" s="7">
         <v>5</v>
       </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="C10" s="6">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F9" s="8">
-        <v>41766</v>
-      </c>
-      <c r="G9" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="7">
-        <v>6</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0.25</v>
-      </c>
       <c r="F10" s="8">
-        <v>41767</v>
+        <f>F9+1</f>
+        <v>41796</v>
       </c>
       <c r="G10" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B11" s="7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
       </c>
       <c r="E11" s="9">
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="F11" s="8">
-        <v>41768</v>
+        <f t="shared" ref="F11:F24" si="1">F10+1</f>
+        <v>41797</v>
       </c>
       <c r="G11" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="7">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F12" s="8">
+        <f>F11+5</f>
+        <v>41802</v>
+      </c>
+      <c r="G12" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>124</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B13" s="7">
         <v>7.5</v>
       </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C13" s="6">
+        <v>0</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F13" s="8">
+        <f>F12+2</f>
+        <v>41804</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="7">
+        <v>8</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0</v>
+      </c>
+      <c r="E14" s="9">
         <v>0.25</v>
       </c>
-      <c r="F12" s="8">
-        <v>41768</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="7">
-        <v>8</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="F13" s="8">
-        <v>41771</v>
-      </c>
-      <c r="G13" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="7">
-        <v>9</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="9">
-        <v>0.5</v>
-      </c>
       <c r="F14" s="8">
-        <v>41772</v>
+        <f>F13+2</f>
+        <v>41806</v>
       </c>
       <c r="G14" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="7">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="6">
         <v>0</v>
       </c>
       <c r="E15" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="8">
-        <v>41772</v>
+        <f t="shared" si="1"/>
+        <v>41807</v>
       </c>
       <c r="G15" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B16" s="7">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="6">
         <v>0</v>
       </c>
       <c r="E16" s="9">
-        <v>0.33333333333333331</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F16" s="8">
-        <v>41773</v>
+        <f t="shared" si="1"/>
+        <v>41808</v>
       </c>
       <c r="G16" s="22">
         <f t="shared" si="0"/>
@@ -1962,19 +2011,20 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="6">
         <v>0</v>
       </c>
       <c r="E17" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F17" s="8">
-        <v>41773</v>
+        <f t="shared" si="1"/>
+        <v>41809</v>
       </c>
       <c r="G17" s="22">
         <f t="shared" si="0"/>
@@ -1983,19 +2033,20 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="7">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="6">
         <v>0</v>
       </c>
       <c r="E18" s="9">
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F18" s="8">
-        <v>41774</v>
+        <f>F17+0</f>
+        <v>41809</v>
       </c>
       <c r="G18" s="22">
         <f t="shared" si="0"/>
@@ -2004,19 +2055,20 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
       </c>
       <c r="E19" s="9">
-        <v>0.66666666666666663</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F19" s="8">
-        <v>41778</v>
+        <f t="shared" si="1"/>
+        <v>41810</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="0"/>
@@ -2025,64 +2077,67 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B20" s="7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6">
         <v>0</v>
       </c>
       <c r="E20" s="9">
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F20" s="8">
-        <v>41781</v>
+        <f>F19+3</f>
+        <v>41813</v>
       </c>
       <c r="G20" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I20" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B21" s="7">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="6">
         <v>0</v>
       </c>
       <c r="E21" s="9">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="F21" s="8">
-        <v>41786</v>
+        <f>F20+3</f>
+        <v>41816</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="I21" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="7">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="6">
         <v>0</v>
       </c>
       <c r="E22" s="9">
-        <v>1.6666666666666667</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F22" s="8">
-        <v>41793</v>
+        <f>F21+4</f>
+        <v>41820</v>
       </c>
       <c r="G22" s="22">
         <f t="shared" si="0"/>
@@ -2091,19 +2146,20 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="6">
         <v>0</v>
       </c>
       <c r="E23" s="9">
-        <v>0.33333333333333331</v>
+        <v>1.6666666666666667</v>
       </c>
       <c r="F23" s="8">
-        <v>41794</v>
+        <f>F22+8</f>
+        <v>41828</v>
       </c>
       <c r="G23" s="22">
         <f t="shared" si="0"/>
@@ -2112,13 +2168,20 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="7">
-        <v>1000</v>
+        <v>18</v>
       </c>
       <c r="C24" s="6">
         <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="1"/>
+        <v>41829</v>
       </c>
       <c r="G24" s="22">
         <f t="shared" si="0"/>
@@ -2127,19 +2190,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="7">
-        <v>19</v>
+        <v>1000</v>
       </c>
       <c r="C25" s="6">
         <v>0</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0.83333333333333337</v>
-      </c>
-      <c r="F25" s="8">
-        <v>41799</v>
       </c>
       <c r="G25" s="22">
         <f t="shared" si="0"/>
@@ -2148,19 +2205,20 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="7">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C26" s="6">
         <v>0</v>
       </c>
       <c r="E26" s="9">
-        <v>0.16666666666666666</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F26" s="8">
-        <v>41799</v>
+        <f>F24+5</f>
+        <v>41834</v>
       </c>
       <c r="G26" s="22">
         <f t="shared" si="0"/>
@@ -2169,10 +2227,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="7">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C27" s="6">
         <v>0</v>
@@ -2181,7 +2239,8 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F27" s="8">
-        <v>41800</v>
+        <f t="shared" ref="F27:F30" si="2">F26+1</f>
+        <v>41835</v>
       </c>
       <c r="G27" s="22">
         <f t="shared" si="0"/>
@@ -2190,19 +2249,20 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="7">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="6">
         <v>0</v>
       </c>
       <c r="E28" s="9">
-        <v>0.25</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="F28" s="8">
-        <v>41801</v>
+        <f t="shared" si="2"/>
+        <v>41836</v>
       </c>
       <c r="G28" s="22">
         <f t="shared" si="0"/>
@@ -2211,19 +2271,20 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="7">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C29" s="6">
         <v>0</v>
       </c>
       <c r="E29" s="9">
-        <v>8.3333333333333329E-2</v>
+        <v>0.25</v>
       </c>
       <c r="F29" s="8">
-        <v>41801</v>
+        <f t="shared" si="2"/>
+        <v>41837</v>
       </c>
       <c r="G29" s="22">
         <f t="shared" si="0"/>
@@ -2232,19 +2293,20 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B30" s="7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="6">
         <v>0</v>
       </c>
       <c r="E30" s="9">
-        <v>1</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="F30" s="8">
-        <v>41806</v>
+        <f t="shared" si="2"/>
+        <v>41838</v>
       </c>
       <c r="G30" s="22">
         <f t="shared" si="0"/>
@@ -2253,19 +2315,20 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C31" s="6">
         <v>0</v>
       </c>
       <c r="E31" s="9">
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="F31" s="8">
-        <v>41809</v>
+        <f>F30+5</f>
+        <v>41843</v>
       </c>
       <c r="G31" s="22">
         <f t="shared" si="0"/>
@@ -2274,21 +2337,44 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B32" s="7">
+        <v>25</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0</v>
+      </c>
+      <c r="E32" s="9">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F32" s="8">
+        <f>F31+3</f>
+        <v>41846</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B33" s="7">
         <v>26</v>
       </c>
-      <c r="C32" s="6">
-        <v>0</v>
-      </c>
-      <c r="E32" s="9">
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="E33" s="9">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F32" s="8">
-        <v>41813</v>
-      </c>
-      <c r="G32" s="22">
+      <c r="F33" s="8">
+        <f>F32+4</f>
+        <v>41850</v>
+      </c>
+      <c r="G33" s="22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2296,5 +2382,8 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="G7 F12" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Text Drawing influenced by View Scale
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1504,16 +1504,16 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="7"/>
-    <col min="3" max="3" width="20.109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="14.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="7.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="22" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
@@ -1791,73 +1791,92 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+    <row r="8" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="18">
         <v>3.6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="19">
         <v>1</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15">
+      <c r="D8" s="19"/>
+      <c r="E8" s="20">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="21">
         <v>41794</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="23">
         <f>SUM(J8:AZ8)</f>
         <v>0.11180555555555555</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="21">
         <v>41794</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="20">
         <v>6.25E-2</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="20">
         <v>4.9305555555555554E-2</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="W8" s="15"/>
-      <c r="X8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="25"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="26"/>
+    </row>
+    <row r="9" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="7">
+      <c r="B9" s="13">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9" s="9">
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="16">
         <f>F8+1</f>
         <v>41795</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="24">
         <f t="shared" ref="G9:G33" si="0">SUM(J9:Y9)</f>
         <v>0</v>
       </c>
+      <c r="H9" s="16"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="25"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" t="s">

</xml_diff>

<commit_message>
Complete: Mouse Over shows world coordinates
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -380,9 +380,6 @@
     <t>Completion Status</t>
   </si>
   <si>
-    <t>Test Coverage</t>
-  </si>
-  <si>
     <t>Time Estimate</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t>Fit View Command</t>
   </si>
   <si>
-    <t>Zoom View</t>
-  </si>
-  <si>
     <t>Apply Features to Elements</t>
   </si>
   <si>
@@ -486,6 +480,13 @@
   </si>
   <si>
     <t>Reimpliment Text draws on View</t>
+  </si>
+  <si>
+    <t>Test
+Coverage</t>
+  </si>
+  <si>
+    <t>Zoom View with Mouse Wheel</t>
   </si>
 </sst>
 </file>
@@ -611,8 +612,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1146,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1500,11 +1503,11 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1512,7 +1515,7 @@
     <col min="1" max="1" width="37.77734375" customWidth="1"/>
     <col min="2" max="2" width="7.5546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="22" customWidth="1"/>
@@ -1523,7 +1526,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E1" s="11">
         <f>SUM(E4:E2003)*24/8</f>
@@ -1534,10 +1537,10 @@
         <v>41810.199999999997</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>82</v>
       </c>
@@ -1547,23 +1550,23 @@
       <c r="C3" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>93</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1689,7 +1692,7 @@
         <v>41762</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J6" s="20">
         <v>0.17361111111111113</v>
@@ -1714,7 +1717,7 @@
     </row>
     <row r="7" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B7" s="18">
         <v>3.5</v>
@@ -1737,7 +1740,7 @@
         <v>41793</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J7" s="20">
         <v>6.25E-2</v>
@@ -1787,13 +1790,13 @@
       <c r="Y7" s="20">
         <v>3.1944444444444449E-2</v>
       </c>
-      <c r="Z7" s="26">
+      <c r="Z7" s="25">
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" s="18">
         <v>3.6</v>
@@ -1810,7 +1813,7 @@
       </c>
       <c r="G8" s="23">
         <f>SUM(J8:AZ8)</f>
-        <v>0.11180555555555555</v>
+        <v>0.12847222222222221</v>
       </c>
       <c r="H8" s="21">
         <v>41794</v>
@@ -1819,7 +1822,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="K8" s="20">
-        <v>4.9305555555555554E-2</v>
+        <v>6.5972222222222224E-2</v>
       </c>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
@@ -1835,70 +1838,98 @@
       <c r="W8" s="20"/>
       <c r="X8" s="20"/>
       <c r="Y8" s="20"/>
-      <c r="Z8" s="26"/>
-    </row>
-    <row r="9" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="Z8" s="25"/>
+    </row>
+    <row r="9" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="18">
         <v>4</v>
       </c>
-      <c r="C9" s="14">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15">
+      <c r="C9" s="19">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20">
         <v>0.20833333333333334</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="21">
         <f>F8+1</f>
         <v>41795</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <f t="shared" ref="G9:G33" si="0">SUM(J9:Y9)</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="16"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
+        <v>0.19027777777777777</v>
+      </c>
+      <c r="H9" s="21">
+        <v>41795</v>
+      </c>
+      <c r="J9" s="20">
+        <v>0.10555555555555556</v>
+      </c>
+      <c r="K9" s="20">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="L9" s="20">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="M9" s="20">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20"/>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
       <c r="Z9" s="25"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="13">
         <v>5</v>
       </c>
-      <c r="C10" s="6">
-        <v>0</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="C10" s="14">
+        <v>0</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="16">
         <f>F9+1</f>
         <v>41796</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15"/>
+      <c r="W10" s="15"/>
+      <c r="X10" s="15"/>
+      <c r="Y10" s="15"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1924,7 +1955,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="7">
         <v>7</v>
@@ -1946,7 +1977,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B13" s="7">
         <v>7.5</v>
@@ -1964,7 +1995,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B14" s="7">
         <v>8</v>
@@ -1986,7 +2017,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="7">
         <v>9</v>
@@ -2008,7 +2039,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B16" s="7">
         <v>10</v>
@@ -2030,7 +2061,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B17" s="7">
         <v>11</v>
@@ -2052,7 +2083,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B18" s="7">
         <v>12</v>
@@ -2074,7 +2105,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B19" s="7">
         <v>13</v>
@@ -2096,7 +2127,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B20" s="7">
         <v>14</v>
@@ -2118,7 +2149,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B21" s="7">
         <v>15</v>
@@ -2138,12 +2169,12 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" s="7">
         <v>16</v>
@@ -2165,7 +2196,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B23" s="7">
         <v>17</v>
@@ -2187,7 +2218,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B24" s="7">
         <v>18</v>
@@ -2209,7 +2240,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B25" s="7">
         <v>1000</v>
@@ -2224,7 +2255,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B26" s="7">
         <v>19</v>
@@ -2246,7 +2277,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B27" s="7">
         <v>20</v>
@@ -2268,7 +2299,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B28" s="7">
         <v>21</v>
@@ -2290,7 +2321,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B29" s="7">
         <v>22</v>
@@ -2312,7 +2343,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B30" s="7">
         <v>23</v>
@@ -2334,7 +2365,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B31" s="7">
         <v>24</v>
@@ -2356,7 +2387,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B32" s="7">
         <v>25</v>
@@ -2378,7 +2409,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B33" s="7">
         <v>26</v>

</xml_diff>

<commit_message>
WIP on Arc class, including Tests
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -377,9 +377,6 @@
     <t>MouseDrag slides View</t>
   </si>
   <si>
-    <t>Completion Status</t>
-  </si>
-  <si>
     <t>Time Estimate</t>
   </si>
   <si>
@@ -487,6 +484,10 @@
   </si>
   <si>
     <t>Zoom View with Mouse Wheel</t>
+  </si>
+  <si>
+    <t>Completion
+Status</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1150,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1503,22 +1504,22 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.77734375" customWidth="1"/>
     <col min="2" max="2" width="7.5546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="6" customWidth="1"/>
     <col min="4" max="4" width="9.5546875" style="6" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" style="9" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="22" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" style="22" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="32.88671875" customWidth="1"/>
     <col min="10" max="25" width="8.88671875" style="9"/>
@@ -1526,7 +1527,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="D1" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E1" s="11">
         <f>SUM(E4:E2003)*24/8</f>
@@ -1537,7 +1538,7 @@
         <v>41810.199999999997</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -1547,26 +1548,26 @@
       <c r="B3" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>97</v>
-      </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
@@ -1692,7 +1693,7 @@
         <v>41762</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J6" s="20">
         <v>0.17361111111111113</v>
@@ -1717,7 +1718,7 @@
     </row>
     <row r="7" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B7" s="18">
         <v>3.5</v>
@@ -1740,7 +1741,7 @@
         <v>41793</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J7" s="20">
         <v>6.25E-2</v>
@@ -1796,7 +1797,7 @@
     </row>
     <row r="8" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B8" s="18">
         <v>3.6</v>
@@ -1899,7 +1900,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="14">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="15">
@@ -1911,12 +1912,18 @@
       </c>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.20763888888888887</v>
       </c>
       <c r="H10" s="16"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="J10" s="15">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="K10" s="15">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="L10" s="15">
+        <v>0.11597222222222221</v>
+      </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15"/>
       <c r="O10" s="15"/>
@@ -1955,7 +1962,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="7">
         <v>7</v>
@@ -1977,7 +1984,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" s="7">
         <v>7.5</v>
@@ -1995,7 +2002,7 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" s="7">
         <v>8</v>
@@ -2017,7 +2024,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B15" s="7">
         <v>9</v>
@@ -2039,7 +2046,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" s="7">
         <v>10</v>
@@ -2061,7 +2068,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="7">
         <v>11</v>
@@ -2083,7 +2090,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="7">
         <v>12</v>
@@ -2105,7 +2112,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="7">
         <v>13</v>
@@ -2127,7 +2134,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B20" s="7">
         <v>14</v>
@@ -2149,7 +2156,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B21" s="7">
         <v>15</v>
@@ -2169,12 +2176,12 @@
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B22" s="7">
         <v>16</v>
@@ -2196,7 +2203,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="7">
         <v>17</v>
@@ -2218,7 +2225,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B24" s="7">
         <v>18</v>
@@ -2240,7 +2247,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B25" s="7">
         <v>1000</v>
@@ -2255,7 +2262,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B26" s="7">
         <v>19</v>
@@ -2277,7 +2284,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B27" s="7">
         <v>20</v>
@@ -2299,7 +2306,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="7">
         <v>21</v>
@@ -2321,7 +2328,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="7">
         <v>22</v>
@@ -2343,7 +2350,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B30" s="7">
         <v>23</v>
@@ -2365,7 +2372,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B31" s="7">
         <v>24</v>
@@ -2387,7 +2394,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B32" s="7">
         <v>25</v>
@@ -2409,7 +2416,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="7">
         <v>26</v>

</xml_diff>

<commit_message>
Arc Class, progress documentation.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1508,7 +1508,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1892,73 +1892,105 @@
       <c r="Y9" s="20"/>
       <c r="Z9" s="25"/>
     </row>
-    <row r="10" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="18">
         <v>5</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="19">
         <v>0.6</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15">
+      <c r="D10" s="19"/>
+      <c r="E10" s="20">
         <v>0.33333333333333331</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="21">
         <f>F9+1</f>
         <v>41796</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="23">
         <f t="shared" si="0"/>
-        <v>0.20763888888888887</v>
-      </c>
-      <c r="H10" s="16"/>
-      <c r="J10" s="15">
+        <v>0.67708333333333326</v>
+      </c>
+      <c r="H10" s="21">
+        <v>41807</v>
+      </c>
+      <c r="J10" s="20">
         <v>7.6388888888888895E-2</v>
       </c>
-      <c r="K10" s="15">
+      <c r="K10" s="20">
         <v>1.5277777777777777E-2</v>
       </c>
-      <c r="L10" s="15">
+      <c r="L10" s="20">
         <v>0.11597222222222221</v>
       </c>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
-      <c r="R10" s="15"/>
-      <c r="S10" s="15"/>
-      <c r="T10" s="15"/>
-      <c r="U10" s="15"/>
-      <c r="V10" s="15"/>
-      <c r="W10" s="15"/>
-      <c r="X10" s="15"/>
-      <c r="Y10" s="15"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="M10" s="20">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="N10" s="20">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="O10" s="20">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="P10" s="20">
+        <v>6.3888888888888884E-2</v>
+      </c>
+      <c r="Q10" s="20">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="R10" s="20">
+        <v>0.20069444444444443</v>
+      </c>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+    </row>
+    <row r="11" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="13">
         <v>6</v>
       </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="C11" s="14">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="15">
         <v>0.25</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="16">
         <f t="shared" ref="F11:F24" si="1">F10+1</f>
         <v>41797</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H11" s="16"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" t="s">

</xml_diff>

<commit_message>
Complete: MouseDrag slides View
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1508,7 +1508,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1952,67 +1952,97 @@
       <c r="X10" s="20"/>
       <c r="Y10" s="20"/>
     </row>
-    <row r="11" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+    <row r="11" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="18">
         <v>6</v>
       </c>
-      <c r="C11" s="14">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15">
+      <c r="C11" s="19">
+        <v>0</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20">
         <v>0.25</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="21">
         <f t="shared" ref="F11:F24" si="1">F10+1</f>
         <v>41797</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="16"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+        <v>0.18680555555555556</v>
+      </c>
+      <c r="H11" s="21">
+        <v>41809</v>
+      </c>
+      <c r="J11" s="20">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="K11" s="20">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="L11" s="20">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="M11" s="20">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="N11" s="20">
+        <v>6.7361111111111108E-2</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="20"/>
+      <c r="U11" s="20"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="20"/>
+      <c r="Y11" s="20"/>
+    </row>
+    <row r="12" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="13">
         <v>7</v>
       </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="C12" s="14">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="15">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="16">
         <f>F11+5</f>
         <v>41802</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H12" s="16"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" t="s">

</xml_diff>

<commit_message>
WIP on Zoom view scale by mouse wheel
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -2006,24 +2006,23 @@
     </row>
     <row r="12" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="B12" s="13">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="C12" s="14">
         <v>0</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="15">
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
       <c r="F12" s="16">
-        <f>F11+5</f>
-        <v>41802</v>
+        <v>41803</v>
       </c>
       <c r="G12" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G12" si="2">SUM(J12:Y12)</f>
         <v>0</v>
       </c>
       <c r="H12" s="16"/>
@@ -2044,44 +2043,62 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="7">
-        <v>7.5</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F13" s="8">
-        <f>F12+2</f>
-        <v>41804</v>
-      </c>
+    <row r="13" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="18">
+        <v>7</v>
+      </c>
+      <c r="C13" s="19">
+        <v>0</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F13" s="21">
+        <f>F11+5</f>
+        <v>41802</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="20"/>
+      <c r="Q13" s="20"/>
+      <c r="R13" s="20"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="20"/>
+      <c r="V13" s="20"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="20"/>
+      <c r="Y13" s="20"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" s="7">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="C14" s="6">
         <v>0</v>
       </c>
       <c r="E14" s="9">
-        <v>0.25</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F14" s="8">
         <f>F13+2</f>
-        <v>41806</v>
-      </c>
-      <c r="G14" s="22">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>41804</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
@@ -2098,8 +2115,8 @@
         <v>0.5</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="1"/>
-        <v>41807</v>
+        <f>F14+1</f>
+        <v>41805</v>
       </c>
       <c r="G15" s="22">
         <f t="shared" si="0"/>
@@ -2121,7 +2138,7 @@
       </c>
       <c r="F16" s="8">
         <f t="shared" si="1"/>
-        <v>41808</v>
+        <v>41806</v>
       </c>
       <c r="G16" s="22">
         <f t="shared" si="0"/>
@@ -2143,7 +2160,7 @@
       </c>
       <c r="F17" s="8">
         <f t="shared" si="1"/>
-        <v>41809</v>
+        <v>41807</v>
       </c>
       <c r="G17" s="22">
         <f t="shared" si="0"/>
@@ -2165,7 +2182,7 @@
       </c>
       <c r="F18" s="8">
         <f>F17+0</f>
-        <v>41809</v>
+        <v>41807</v>
       </c>
       <c r="G18" s="22">
         <f t="shared" si="0"/>
@@ -2187,7 +2204,7 @@
       </c>
       <c r="F19" s="8">
         <f t="shared" si="1"/>
-        <v>41810</v>
+        <v>41808</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="0"/>
@@ -2209,7 +2226,7 @@
       </c>
       <c r="F20" s="8">
         <f>F19+3</f>
-        <v>41813</v>
+        <v>41811</v>
       </c>
       <c r="G20" s="22">
         <f t="shared" si="0"/>
@@ -2231,7 +2248,7 @@
       </c>
       <c r="F21" s="8">
         <f>F20+3</f>
-        <v>41816</v>
+        <v>41814</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="0"/>
@@ -2256,7 +2273,7 @@
       </c>
       <c r="F22" s="8">
         <f>F21+4</f>
-        <v>41820</v>
+        <v>41818</v>
       </c>
       <c r="G22" s="22">
         <f t="shared" si="0"/>
@@ -2278,7 +2295,7 @@
       </c>
       <c r="F23" s="8">
         <f>F22+8</f>
-        <v>41828</v>
+        <v>41826</v>
       </c>
       <c r="G23" s="22">
         <f t="shared" si="0"/>
@@ -2300,7 +2317,7 @@
       </c>
       <c r="F24" s="8">
         <f t="shared" si="1"/>
-        <v>41829</v>
+        <v>41827</v>
       </c>
       <c r="G24" s="22">
         <f t="shared" si="0"/>
@@ -2337,7 +2354,7 @@
       </c>
       <c r="F26" s="8">
         <f>F24+5</f>
-        <v>41834</v>
+        <v>41832</v>
       </c>
       <c r="G26" s="22">
         <f t="shared" si="0"/>
@@ -2358,8 +2375,8 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F27" s="8">
-        <f t="shared" ref="F27:F30" si="2">F26+1</f>
-        <v>41835</v>
+        <f t="shared" ref="F27:F30" si="3">F26+1</f>
+        <v>41833</v>
       </c>
       <c r="G27" s="22">
         <f t="shared" si="0"/>
@@ -2380,8 +2397,8 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="F28" s="8">
-        <f t="shared" si="2"/>
-        <v>41836</v>
+        <f t="shared" si="3"/>
+        <v>41834</v>
       </c>
       <c r="G28" s="22">
         <f t="shared" si="0"/>
@@ -2402,8 +2419,8 @@
         <v>0.25</v>
       </c>
       <c r="F29" s="8">
-        <f t="shared" si="2"/>
-        <v>41837</v>
+        <f t="shared" si="3"/>
+        <v>41835</v>
       </c>
       <c r="G29" s="22">
         <f t="shared" si="0"/>
@@ -2424,8 +2441,8 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="F30" s="8">
-        <f t="shared" si="2"/>
-        <v>41838</v>
+        <f t="shared" si="3"/>
+        <v>41836</v>
       </c>
       <c r="G30" s="22">
         <f t="shared" si="0"/>
@@ -2447,7 +2464,7 @@
       </c>
       <c r="F31" s="8">
         <f>F30+5</f>
-        <v>41843</v>
+        <v>41841</v>
       </c>
       <c r="G31" s="22">
         <f t="shared" si="0"/>
@@ -2469,7 +2486,7 @@
       </c>
       <c r="F32" s="8">
         <f>F31+3</f>
-        <v>41846</v>
+        <v>41844</v>
       </c>
       <c r="G32" s="22">
         <f t="shared" si="0"/>
@@ -2491,7 +2508,7 @@
       </c>
       <c r="F33" s="8">
         <f>F32+4</f>
-        <v>41850</v>
+        <v>41848</v>
       </c>
       <c r="G33" s="22">
         <f t="shared" si="0"/>
@@ -2502,7 +2519,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="G7 F12" formula="1"/>
+    <ignoredError sqref="G7 F13" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete: Zoom view scale by mouse wheel
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1504,11 +1504,11 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2004,84 +2004,88 @@
       <c r="X11" s="20"/>
       <c r="Y11" s="20"/>
     </row>
-    <row r="12" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+    <row r="12" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
         <v>125</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="18">
         <v>6.5</v>
       </c>
-      <c r="C12" s="14">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="15">
+      <c r="C12" s="19">
+        <v>0</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20">
         <v>0.25</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="21">
         <v>41803</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="23">
         <f t="shared" ref="G12" si="2">SUM(J12:Y12)</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="16"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-    </row>
-    <row r="13" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="H12" s="21">
+        <v>41814</v>
+      </c>
+      <c r="J12" s="20">
+        <v>0.22847222222222222</v>
+      </c>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="20"/>
+      <c r="W12" s="20"/>
+      <c r="X12" s="20"/>
+      <c r="Y12" s="20"/>
+    </row>
+    <row r="13" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="13">
         <v>7</v>
       </c>
-      <c r="C13" s="19">
-        <v>0</v>
-      </c>
-      <c r="D13" s="19"/>
-      <c r="E13" s="20">
+      <c r="C13" s="14">
+        <v>0</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="15">
         <v>0.16666666666666666</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="16">
         <f>F11+5</f>
         <v>41802</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="20"/>
-      <c r="V13" s="20"/>
-      <c r="W13" s="20"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
+      <c r="H13" s="16"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" t="s">

</xml_diff>

<commit_message>
WIP Apply Features to Elements
Implemented Transparency for LineSegments and Arcs.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -493,7 +493,7 @@
     <t>Skipped.  Will return later.</t>
   </si>
   <si>
-    <t>Only implmntd Name, Style, Weight, Thickness, DisplayPriority</t>
+    <t>Only implmntd Name, Style, Weight, Thickness, DisplayPriority, Transparency</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Complete: Apply Features to Elements
Now implemented for text items.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1510,11 +1510,11 @@
   <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2097,75 +2097,100 @@
       <c r="X13" s="20"/>
       <c r="Y13" s="20"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="14" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="13">
         <v>7.5</v>
       </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="9">
+      <c r="C14" s="14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="15">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="16">
         <f>F13+2</f>
         <v>41804</v>
       </c>
-      <c r="I14" t="s">
+      <c r="G14" s="24"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="12" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15"/>
+      <c r="W14" s="15"/>
+      <c r="X14" s="15"/>
+      <c r="Y14" s="15"/>
+    </row>
+    <row r="15" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="18">
         <v>9</v>
       </c>
-      <c r="C15" s="14">
-        <v>0</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15">
+      <c r="C15" s="19">
+        <v>0</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20">
         <v>0.5</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="21">
         <f>F14+1</f>
         <v>41805</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="23">
         <f t="shared" si="0"/>
-        <v>0.31805555555555559</v>
-      </c>
-      <c r="H15" s="16"/>
-      <c r="I15" s="12" t="s">
+        <v>0.51666666666666672</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="20">
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="K15" s="15">
+      <c r="K15" s="20">
         <v>0.1277777777777778</v>
       </c>
-      <c r="L15" s="15">
+      <c r="L15" s="20">
         <v>0.17361111111111113</v>
       </c>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
+      <c r="M15" s="20">
+        <v>0.10694444444444444</v>
+      </c>
+      <c r="N15" s="20">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="O15" s="20">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="P15" s="20"/>
+      <c r="Q15" s="20"/>
+      <c r="R15" s="20"/>
+      <c r="S15" s="20"/>
+      <c r="T15" s="20"/>
+      <c r="U15" s="20"/>
+      <c r="V15" s="20"/>
+      <c r="W15" s="20"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Rotated views: elements, coordinate xfrms
Started and Finished, all 3 types of elements currently supported.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -490,10 +490,10 @@
 Status</t>
   </si>
   <si>
-    <t>Skipped.  Will return later.</t>
-  </si>
-  <si>
     <t>Only implmntd Name, Style, Weight, Thickness, DisplayPriority, Transparency</t>
+  </si>
+  <si>
+    <t>That was easy.</t>
   </si>
 </sst>
 </file>
@@ -1514,7 +1514,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2097,45 +2097,52 @@
       <c r="X13" s="20"/>
       <c r="Y13" s="20"/>
     </row>
-    <row r="14" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="18">
         <v>7.5</v>
       </c>
-      <c r="C14" s="14">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15">
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="21">
         <f>F13+2</f>
         <v>41804</v>
       </c>
-      <c r="G14" s="24"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
+      <c r="G14" s="23">
+        <f t="shared" si="0"/>
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H14" s="21">
+        <v>41816</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="J14" s="20">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="K14" s="20"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
     </row>
     <row r="15" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
@@ -2157,11 +2164,13 @@
       </c>
       <c r="G15" s="23">
         <f t="shared" si="0"/>
-        <v>0.51666666666666672</v>
-      </c>
-      <c r="H15" s="21"/>
+        <v>0.51597222222222228</v>
+      </c>
+      <c r="H15" s="21">
+        <v>41816</v>
+      </c>
       <c r="I15" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J15" s="20">
         <v>1.6666666666666666E-2</v>
@@ -2179,7 +2188,7 @@
         <v>7.9861111111111105E-2</v>
       </c>
       <c r="O15" s="20">
-        <v>1.1805555555555555E-2</v>
+        <v>1.1111111111111112E-2</v>
       </c>
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
@@ -2192,27 +2201,45 @@
       <c r="X15" s="20"/>
       <c r="Y15" s="20"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="16" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="13">
         <v>10</v>
       </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
+      <c r="C16" s="14">
+        <v>0</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="15">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="16">
         <f t="shared" si="1"/>
         <v>41806</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H16" s="16"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">

</xml_diff>

<commit_message>
+Tooltip box for linesegment, arc, and text.
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1520,7 +1520,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2207,87 +2207,87 @@
       <c r="X15" s="20"/>
       <c r="Y15" s="20"/>
     </row>
-    <row r="16" spans="1:26" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:26" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="18">
         <v>9.5</v>
       </c>
-      <c r="C16" s="14">
-        <v>0</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15">
+      <c r="C16" s="19">
+        <v>0</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="21">
         <v>41806</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16" s="23">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H16" s="21">
+        <v>41816</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="20"/>
+      <c r="Q16" s="20"/>
+      <c r="R16" s="20"/>
+      <c r="S16" s="20"/>
+      <c r="T16" s="20"/>
+      <c r="U16" s="20"/>
+      <c r="V16" s="20"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="20"/>
+      <c r="Y16" s="20"/>
+    </row>
+    <row r="17" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="13">
+        <v>10</v>
+      </c>
+      <c r="C17" s="14">
+        <v>0</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="15">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F17" s="16">
+        <v>41978</v>
+      </c>
+      <c r="G17" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="16"/>
-      <c r="I16" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-    </row>
-    <row r="17" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="18">
-        <v>10</v>
-      </c>
-      <c r="C17" s="19">
-        <v>0</v>
-      </c>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20">
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="F17" s="21">
-        <f>F15+1</f>
-        <v>41806</v>
-      </c>
-      <c r="G17" s="23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="21"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="20"/>
-      <c r="U17" s="20"/>
-      <c r="V17" s="20"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="20"/>
-      <c r="Y17" s="20"/>
+      <c r="H17" s="16"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="15"/>
+      <c r="X17" s="15"/>
+      <c r="Y17" s="15"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
@@ -2304,7 +2304,7 @@
       </c>
       <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>41807</v>
+        <v>41979</v>
       </c>
       <c r="G18" s="22">
         <f t="shared" si="0"/>
@@ -2326,7 +2326,7 @@
       </c>
       <c r="F19" s="8">
         <f>F18+0</f>
-        <v>41807</v>
+        <v>41979</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="0"/>
@@ -2348,7 +2348,7 @@
       </c>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>41808</v>
+        <v>41980</v>
       </c>
       <c r="G20" s="22">
         <f t="shared" si="0"/>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="F21" s="8">
         <f>F20+3</f>
-        <v>41811</v>
+        <v>41983</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="0"/>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="F22" s="8">
         <f>F21+3</f>
-        <v>41814</v>
+        <v>41986</v>
       </c>
       <c r="G22" s="22">
         <f t="shared" si="0"/>
@@ -2417,7 +2417,7 @@
       </c>
       <c r="F23" s="8">
         <f>F22+4</f>
-        <v>41818</v>
+        <v>41990</v>
       </c>
       <c r="G23" s="22">
         <f t="shared" si="0"/>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="F24" s="8">
         <f>F23+8</f>
-        <v>41826</v>
+        <v>41998</v>
       </c>
       <c r="G24" s="22">
         <f t="shared" si="0"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="F25" s="8">
         <f t="shared" si="1"/>
-        <v>41827</v>
+        <v>41999</v>
       </c>
       <c r="G25" s="22">
         <f t="shared" si="0"/>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="F27" s="8">
         <f>F25+5</f>
-        <v>41832</v>
+        <v>42004</v>
       </c>
       <c r="G27" s="22">
         <f t="shared" si="0"/>
@@ -2520,7 +2520,7 @@
       </c>
       <c r="F28" s="8">
         <f t="shared" ref="F28:F31" si="3">F27+1</f>
-        <v>41833</v>
+        <v>42005</v>
       </c>
       <c r="G28" s="22">
         <f t="shared" si="0"/>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="F29" s="8">
         <f t="shared" si="3"/>
-        <v>41834</v>
+        <v>42006</v>
       </c>
       <c r="G29" s="22">
         <f t="shared" si="0"/>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="F30" s="8">
         <f t="shared" si="3"/>
-        <v>41835</v>
+        <v>42007</v>
       </c>
       <c r="G30" s="22">
         <f t="shared" si="0"/>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="F31" s="8">
         <f t="shared" si="3"/>
-        <v>41836</v>
+        <v>42008</v>
       </c>
       <c r="G31" s="22">
         <f t="shared" si="0"/>
@@ -2608,7 +2608,7 @@
       </c>
       <c r="F32" s="8">
         <f>F31+5</f>
-        <v>41841</v>
+        <v>42013</v>
       </c>
       <c r="G32" s="22">
         <f t="shared" si="0"/>
@@ -2630,7 +2630,7 @@
       </c>
       <c r="F33" s="8">
         <f>F32+3</f>
-        <v>41844</v>
+        <v>42016</v>
       </c>
       <c r="G33" s="22">
         <f t="shared" si="0"/>
@@ -2652,7 +2652,7 @@
       </c>
       <c r="F34" s="8">
         <f>F33+4</f>
-        <v>41848</v>
+        <v>42020</v>
       </c>
       <c r="G34" s="22">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
+Create Model from DXF: Load Features from Layers
</commit_message>
<xml_diff>
--- a/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
+++ b/ProjectManagement/ImplementationList_FoundationClassHierarchy.xlsx
@@ -1520,7 +1520,7 @@
       <selection activeCell="J1" sqref="J1"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2225,6 +2225,7 @@
         <v>41806</v>
       </c>
       <c r="G16" s="23">
+        <f t="shared" si="0"/>
         <v>2.013888888888889E-2</v>
       </c>
       <c r="H16" s="21">
@@ -2233,7 +2234,9 @@
       <c r="I16" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="J16" s="20"/>
+      <c r="J16" s="20">
+        <v>2.013888888888889E-2</v>
+      </c>
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
       <c r="M16" s="20"/>
@@ -2250,66 +2253,88 @@
       <c r="X16" s="20"/>
       <c r="Y16" s="20"/>
     </row>
-    <row r="17" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+    <row r="17" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="18">
         <v>10</v>
       </c>
-      <c r="C17" s="14">
-        <v>0</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15">
+      <c r="C17" s="19">
+        <v>0</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="21">
         <v>41978</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="23">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H17" s="16"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="15"/>
-      <c r="L17" s="15"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="15"/>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="15"/>
-      <c r="S17" s="15"/>
-      <c r="T17" s="15"/>
-      <c r="U17" s="15"/>
-      <c r="V17" s="15"/>
-      <c r="W17" s="15"/>
-      <c r="X17" s="15"/>
-      <c r="Y17" s="15"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="H17" s="21">
+        <v>41978</v>
+      </c>
+      <c r="J17" s="20">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="K17" s="20"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="20"/>
+      <c r="R17" s="20"/>
+      <c r="S17" s="20"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="20"/>
+      <c r="W17" s="20"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="20"/>
+    </row>
+    <row r="18" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="13">
         <v>11</v>
       </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18" s="9">
+      <c r="C18" s="14">
+        <v>0</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="15">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F18" s="8">
-        <f t="shared" si="1"/>
-        <v>41979</v>
-      </c>
-      <c r="G18" s="22">
+      <c r="F18" s="16">
+        <f>F17+24*E18/8</f>
+        <v>41980</v>
+      </c>
+      <c r="G18" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H18" s="16"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="15"/>
+      <c r="Y18" s="15"/>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
@@ -2326,7 +2351,7 @@
       </c>
       <c r="F19" s="8">
         <f>F18+0</f>
-        <v>41979</v>
+        <v>41980</v>
       </c>
       <c r="G19" s="22">
         <f t="shared" si="0"/>
@@ -2348,7 +2373,7 @@
       </c>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>41980</v>
+        <v>41981</v>
       </c>
       <c r="G20" s="22">
         <f t="shared" si="0"/>
@@ -2370,7 +2395,7 @@
       </c>
       <c r="F21" s="8">
         <f>F20+3</f>
-        <v>41983</v>
+        <v>41984</v>
       </c>
       <c r="G21" s="22">
         <f t="shared" si="0"/>
@@ -2392,7 +2417,7 @@
       </c>
       <c r="F22" s="8">
         <f>F21+3</f>
-        <v>41986</v>
+        <v>41987</v>
       </c>
       <c r="G22" s="22">
         <f t="shared" si="0"/>
@@ -2417,7 +2442,7 @@
       </c>
       <c r="F23" s="8">
         <f>F22+4</f>
-        <v>41990</v>
+        <v>41991</v>
       </c>
       <c r="G23" s="22">
         <f t="shared" si="0"/>
@@ -2439,7 +2464,7 @@
       </c>
       <c r="F24" s="8">
         <f>F23+8</f>
-        <v>41998</v>
+        <v>41999</v>
       </c>
       <c r="G24" s="22">
         <f t="shared" si="0"/>
@@ -2461,7 +2486,7 @@
       </c>
       <c r="F25" s="8">
         <f t="shared" si="1"/>
-        <v>41999</v>
+        <v>42000</v>
       </c>
       <c r="G25" s="22">
         <f t="shared" si="0"/>
@@ -2498,7 +2523,7 @@
       </c>
       <c r="F27" s="8">
         <f>F25+5</f>
-        <v>42004</v>
+        <v>42005</v>
       </c>
       <c r="G27" s="22">
         <f t="shared" si="0"/>
@@ -2520,7 +2545,7 @@
       </c>
       <c r="F28" s="8">
         <f t="shared" ref="F28:F31" si="3">F27+1</f>
-        <v>42005</v>
+        <v>42006</v>
       </c>
       <c r="G28" s="22">
         <f t="shared" si="0"/>
@@ -2542,7 +2567,7 @@
       </c>
       <c r="F29" s="8">
         <f t="shared" si="3"/>
-        <v>42006</v>
+        <v>42007</v>
       </c>
       <c r="G29" s="22">
         <f t="shared" si="0"/>
@@ -2564,7 +2589,7 @@
       </c>
       <c r="F30" s="8">
         <f t="shared" si="3"/>
-        <v>42007</v>
+        <v>42008</v>
       </c>
       <c r="G30" s="22">
         <f t="shared" si="0"/>
@@ -2586,7 +2611,7 @@
       </c>
       <c r="F31" s="8">
         <f t="shared" si="3"/>
-        <v>42008</v>
+        <v>42009</v>
       </c>
       <c r="G31" s="22">
         <f t="shared" si="0"/>
@@ -2608,7 +2633,7 @@
       </c>
       <c r="F32" s="8">
         <f>F31+5</f>
-        <v>42013</v>
+        <v>42014</v>
       </c>
       <c r="G32" s="22">
         <f t="shared" si="0"/>
@@ -2630,7 +2655,7 @@
       </c>
       <c r="F33" s="8">
         <f>F32+3</f>
-        <v>42016</v>
+        <v>42017</v>
       </c>
       <c r="G33" s="22">
         <f t="shared" si="0"/>
@@ -2652,7 +2677,7 @@
       </c>
       <c r="F34" s="8">
         <f>F33+4</f>
-        <v>42020</v>
+        <v>42021</v>
       </c>
       <c r="G34" s="22">
         <f t="shared" si="0"/>

</xml_diff>